<commit_message>
Done with first draft
</commit_message>
<xml_diff>
--- a/api/result/excel/rf-antidp-chem-plus-pheno-pred-bio (f cutoff 0.1716385) (highlight) (weighted) (1-known, 2-predict, 3-validated).xlsx
+++ b/api/result/excel/rf-antidp-chem-plus-pheno-pred-bio (f cutoff 0.1716385) (highlight) (weighted) (1-known, 2-predict, 3-validated).xlsx
@@ -4273,8 +4273,8 @@
   <dimension ref="A1:ALC17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AKU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AKI17" sqref="AKI17"/>
+      <pane xSplit="2" topLeftCell="CM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CN17" sqref="CN17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -25402,10 +25402,10 @@
         <v>0</v>
       </c>
       <c r="CN8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CO8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CP8">
         <v>0</v>

</xml_diff>